<commit_message>
WiP: Tests for erillishaun tuonti
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku_uusilla_kentilla.xlsx
+++ b/src/test/resources/erillishaku_uusilla_kentilla.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessika/dev/oph/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harri.hamalainen/code/oph/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34580" yWindow="2420" windowWidth="27700" windowHeight="17540"/>
+    <workbookView xWindow="120" yWindow="4780" windowWidth="27700" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Erillishaku" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
-  <si>
-    <t>Rakennusalan perustutkinto</t>
-  </si>
-  <si>
-    <t>Tampereen Aikuiskoulutuskeskus</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Sukunimi</t>
   </si>
@@ -139,7 +133,13 @@
     <t>FIN</t>
   </si>
   <si>
-    <t>091</t>
+    <t>EI_TEHTY</t>
+  </si>
+  <si>
+    <t>Julkaistavissa</t>
+  </si>
+  <si>
+    <t>Helsinki</t>
   </si>
 </sst>
 </file>
@@ -177,49 +177,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -243,20 +206,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1581,327 +1543,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IS10"/>
+  <dimension ref="A1:IT2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="253" width="8.125" style="1" customWidth="1"/>
+    <col min="1" max="13" width="8.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.125" style="5" customWidth="1"/>
+    <col min="15" max="254" width="8.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
+    <row r="1" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="2"/>
+    <row r="2" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-    </row>
-    <row r="3" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-    </row>
-    <row r="4" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S5" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="8" t="s">
+      <c r="Q2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="S2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-    </row>
-    <row r="9" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-    </row>
-    <row r="10" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
+      <c r="U2" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="25" orientation="portrait"/>

</xml_diff>